<commit_message>
update 22127444: infor + evaluate + bug report
</commit_message>
<xml_diff>
--- a/project/HW2/22127444/22127444_DomainTesting_10/22127444_Bug Report.xlsx
+++ b/project/HW2/22127444/22127444_DomainTesting_10/22127444_Bug Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\Testing-PRJ-SM\project\HW2\22127444\release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\Testing-PRJ-SM\project\HW2\22127444\22127444_DomainTesting_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BBE5CA-A716-4108-B3AE-9340A1C0C997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ABE9F6-8A2F-4CF8-A432-7F9BC4D82940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
   <si>
     <t>Tester</t>
   </si>
@@ -386,6 +386,60 @@
   <si>
     <t>1. Message not sent
 2. Warning "Message is required"</t>
+  </si>
+  <si>
+    <t>Search with space keyword</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>No category show</t>
+  </si>
+  <si>
+    <t>All categories listed</t>
+  </si>
+  <si>
+    <t>Add with uppercase slug</t>
+  </si>
+  <si>
+    <t>Error: Slug cannot contain spaces</t>
+  </si>
+  <si>
+    <t>Error: Slug must be lowercase</t>
+  </si>
+  <si>
+    <t>Add category with existing name, different slug</t>
+  </si>
+  <si>
+    <t>Error message displayed</t>
+  </si>
+  <si>
+    <t>Error: Name must be unique</t>
+  </si>
+  <si>
+    <t>Add with name containing newline</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Category added successfully</t>
+  </si>
+  <si>
+    <t>Likely error due to newline</t>
+  </si>
+  <si>
+    <t>B016</t>
+  </si>
+  <si>
+    <t>B017</t>
+  </si>
+  <si>
+    <t>B018</t>
+  </si>
+  <si>
+    <t>B019</t>
   </si>
 </sst>
 </file>
@@ -463,6 +517,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -475,7 +530,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -516,21 +570,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:M16" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:M20" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Bug ID" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Summary" dataDxfId="11"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Steps to Reproduce" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{B3FD4646-B743-4A31-B82D-F63B189E8DDD}" name="Actual Result" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{BF8CDC4F-F23B-4D30-9802-B965224E4AEE}" name="Expected Result" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{AB022B76-AC97-4D7C-A725-6DC5682042BB}" name="Priority" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Function ID" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Severity" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{C82857A7-A27E-4F8A-8D4F-68111ED2442C}" name="Affected Feature / Version" dataDxfId="0"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Reported By" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date Reported" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Status" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B3FD4646-B743-4A31-B82D-F63B189E8DDD}" name="Actual Result" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{BF8CDC4F-F23B-4D30-9802-B965224E4AEE}" name="Expected Result" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{AB022B76-AC97-4D7C-A725-6DC5682042BB}" name="Priority" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Function ID" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Severity" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{C82857A7-A27E-4F8A-8D4F-68111ED2442C}" name="Affected Feature / Version" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Reported By" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date Reported" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -869,10 +923,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -884,7 +938,7 @@
     <col min="7" max="7" width="12.46484375" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.59765625" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.3984375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.19921875" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.796875" style="1" customWidth="1"/>
     <col min="12" max="12" width="16.796875" style="1" customWidth="1"/>
     <col min="13" max="13" width="28.1328125" style="1" customWidth="1"/>
@@ -1504,6 +1558,158 @@
         <v>10</v>
       </c>
     </row>
+    <row r="17" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="4">
+        <v>45819</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="4">
+        <v>45819</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="4">
+        <v>45819</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="4">
+        <v>45819</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>